<commit_message>
add auth simple examples
</commit_message>
<xml_diff>
--- a/docs/table-ddl.xlsx
+++ b/docs/table-ddl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/idea-workspace/other/github/dubbo-nacos/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CE2DEB-C79C-8B4A-9152-210904FE3524}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2964C28C-7D47-4F41-B39E-EE421467F10E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19100" tabRatio="611" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19100" tabRatio="611" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="表设计" sheetId="2" r:id="rId1"/>
@@ -74,10 +74,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>permission</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>bigint(19)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -142,10 +138,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>role</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Role</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -194,10 +186,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>role_permission</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Role Permission</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -222,10 +210,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>user</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>User</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -282,10 +266,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>user_role</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>User Role</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -750,6 +730,26 @@
   </si>
   <si>
     <t>varchar(200)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dn_permission</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dn_role</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dn_role_permission</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dn_user</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dn_user_role</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1217,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:G134"/>
+  <dimension ref="A3:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
@@ -1244,10 +1244,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>187</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>6</v>
@@ -1307,7 +1307,7 @@
     ""
     )
 )</f>
-        <v>CREATE TABLE `permission` (</v>
+        <v>CREATE TABLE `dn_permission` (</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1315,12 +1315,12 @@
         <v>0</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="15" t="str">
@@ -1365,15 +1365,15 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="15" t="str">
@@ -1418,17 +1418,17 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="15" t="str">
@@ -1473,7 +1473,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>2</v>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="15" t="str">
@@ -1528,17 +1528,17 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="15" t="str">
@@ -1583,17 +1583,17 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="12" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="15" t="str">
@@ -1638,17 +1638,17 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="15" t="str">
@@ -1693,17 +1693,17 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="15" t="str">
@@ -1748,17 +1748,17 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="15" t="str">
@@ -1896,12 +1896,15 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="G17" s="15" t="str">
         <f>IF(
     A17="Column",
@@ -1943,15 +1946,22 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="7"/>
       <c r="G18" s="15" t="str">
         <f>IF(
     A18="Column",
@@ -1989,26 +1999,22 @@
     ""
     )
 )</f>
-        <v/>
+        <v>CREATE TABLE `dn_role` (</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="7"/>
+      <c r="A19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="10"/>
       <c r="G19" s="15" t="str">
         <f>IF(
     A19="Column",
@@ -2046,20 +2052,20 @@
     ""
     )
 )</f>
-        <v>CREATE TABLE `role` (</v>
+        <v xml:space="preserve">   `id` bigint(19)  NOT NULL  COMMENT 'Pk',</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="8" t="s">
-        <v>0</v>
+      <c r="A20" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="15" t="str">
@@ -2099,20 +2105,20 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `id` bigint(19)  NOT NULL  COMMENT 'Pk',</v>
+        <v xml:space="preserve">   `role_name` varchar(20)  NOT NULL  COMMENT 'role name',</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="15" t="str">
@@ -2152,7 +2158,7 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `role_name` varchar(20)  NOT NULL  COMMENT 'role name',</v>
+        <v xml:space="preserve">   `role_code` varchar(25)  NOT NULL  COMMENT 'role code',</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2160,12 +2166,14 @@
         <v>30</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>5</v>
+      </c>
       <c r="D22" s="9"/>
       <c r="E22" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="15" t="str">
@@ -2205,22 +2213,22 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `role_code` varchar(25)  NOT NULL  COMMENT 'role code',</v>
+        <v xml:space="preserve">   `parent_id` bigint(19)  COMMENT 'parent role id',</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="15" t="str">
@@ -2260,22 +2268,22 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `parent_id` bigint(19)  COMMENT 'parent role id',</v>
+        <v xml:space="preserve">   `role_type` varchar(8)  COMMENT 'role type',</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="12" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="15" t="str">
@@ -2315,24 +2323,10 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `role_type` varchar(8)  COMMENT 'role type',</v>
+        <v xml:space="preserve">   `remark` varchar(255)  COMMENT 'role remark',</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="10"/>
       <c r="G25" s="15" t="str">
         <f>IF(
     A25="Column",
@@ -2370,7 +2364,7 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `remark` varchar(255)  COMMENT 'role remark',</v>
+        <v xml:space="preserve">   PRIMARY KEY(`id`)</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2411,10 +2405,19 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   PRIMARY KEY(`id`)</v>
+        <v>) ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='Role';</v>
       </c>
     </row>
     <row r="27" spans="1:7">
+      <c r="A27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="G27" s="15" t="str">
         <f>IF(
     A27="Column",
@@ -2452,10 +2455,26 @@
     ""
     )
 )</f>
-        <v>) ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='Role';</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:7">
+      <c r="A28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="7"/>
       <c r="G28" s="15" t="str">
         <f>IF(
     A28="Column",
@@ -2493,19 +2512,22 @@
     ""
     )
 )</f>
-        <v/>
+        <v>CREATE TABLE `dn_role_permission` (</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="A29" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="10"/>
       <c r="G29" s="15" t="str">
         <f>IF(
     A29="Column",
@@ -2543,26 +2565,22 @@
     ""
     )
 )</f>
-        <v/>
+        <v xml:space="preserve">   `id` bigint(19)  NOT NULL  COMMENT 'Pk',</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="7"/>
+      <c r="A30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="10"/>
       <c r="G30" s="15" t="str">
         <f>IF(
     A30="Column",
@@ -2600,20 +2618,22 @@
     ""
     )
 )</f>
-        <v>CREATE TABLE `role_permission` (</v>
+        <v xml:space="preserve">   `role_id` bigint(19)  NOT NULL  COMMENT 'role id',</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="8" t="s">
-        <v>0</v>
+      <c r="A31" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="15" t="str">
@@ -2653,20 +2673,20 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `id` bigint(19)  NOT NULL  COMMENT 'Pk',</v>
+        <v xml:space="preserve">   `permission_id` bigint(19)  COMMENT 'permission id',</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="12" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="15" t="str">
@@ -2706,24 +2726,10 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `role_id` bigint(19)  NOT NULL  COMMENT 'role id',</v>
+        <v xml:space="preserve">   `site_code` varchar(20)  NOT NULL  COMMENT 'site type',</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" s="10"/>
       <c r="G33" s="15" t="str">
         <f>IF(
     A33="Column",
@@ -2761,22 +2767,10 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `permission_id` bigint(19)  COMMENT 'permission id',</v>
+        <v xml:space="preserve">   PRIMARY KEY(`id`)</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" s="10"/>
       <c r="G34" s="15" t="str">
         <f>IF(
     A34="Column",
@@ -2814,10 +2808,19 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `site_code` varchar(20)  NOT NULL  COMMENT 'site type',</v>
+        <v>) ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='Role Permission';</v>
       </c>
     </row>
     <row r="35" spans="1:7">
+      <c r="A35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G35" s="15" t="str">
         <f>IF(
     A35="Column",
@@ -2855,10 +2858,26 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   PRIMARY KEY(`id`)</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:7">
+      <c r="A36" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="7"/>
       <c r="G36" s="15" t="str">
         <f>IF(
     A36="Column",
@@ -2896,10 +2915,22 @@
     ""
     )
 )</f>
-        <v>) ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='Role Permission';</v>
+        <v>CREATE TABLE `dn_user` (</v>
       </c>
     </row>
     <row r="37" spans="1:7">
+      <c r="A37" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="10"/>
       <c r="G37" s="15" t="str">
         <f>IF(
     A37="Column",
@@ -2937,19 +2968,22 @@
     ""
     )
 )</f>
-        <v/>
+        <v xml:space="preserve">   `id` bigint(19)  NOT NULL  COMMENT 'Pk',</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="A38" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="10"/>
       <c r="G38" s="15" t="str">
         <f>IF(
     A38="Column",
@@ -2987,26 +3021,22 @@
     ""
     )
 )</f>
-        <v/>
+        <v xml:space="preserve">   `account` varchar(20)  NOT NULL  COMMENT 'user login account',</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="7"/>
+      <c r="A39" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="10"/>
       <c r="G39" s="15" t="str">
         <f>IF(
     A39="Column",
@@ -3044,20 +3074,20 @@
     ""
     )
 )</f>
-        <v>CREATE TABLE `user` (</v>
+        <v xml:space="preserve">   `password` varchar(200)  NOT NULL  COMMENT 'user login password',</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="8" t="s">
-        <v>0</v>
+      <c r="A40" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="12" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="15" t="str">
@@ -3097,20 +3127,22 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `id` bigint(19)  NOT NULL  COMMENT 'Pk',</v>
+        <v xml:space="preserve">   `real_name` varchar(20)  NOT NULL  COMMENT 'user real name',</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="D41" s="9"/>
       <c r="E41" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="15" t="str">
@@ -3150,20 +3182,22 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `account` varchar(20)  NOT NULL  COMMENT 'user login account',</v>
+        <v xml:space="preserve">   `email` varchar(50)  COMMENT 'user email',</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C42" s="9"/>
+        <v>58</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="D42" s="9"/>
       <c r="E42" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="15" t="str">
@@ -3203,20 +3237,22 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `password` varchar(200)  NOT NULL  COMMENT 'user login password',</v>
+        <v xml:space="preserve">   `mobile` int(15)  COMMENT 'user mobile',</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="D43" s="9"/>
       <c r="E43" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="15" t="str">
@@ -3256,24 +3292,10 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `real_name` varchar(20)  NOT NULL  COMMENT 'user real name',</v>
+        <v xml:space="preserve">   `salt` varchar(100)  COMMENT 'salt code ',</v>
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F44" s="10"/>
       <c r="G44" s="15" t="str">
         <f>IF(
     A44="Column",
@@ -3311,24 +3333,10 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `email` varchar(50)  COMMENT 'user email',</v>
+        <v xml:space="preserve">   PRIMARY KEY(`id`)</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" s="10"/>
       <c r="G45" s="15" t="str">
         <f>IF(
     A45="Column",
@@ -3366,24 +3374,19 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `mobile` int(15)  COMMENT 'user mobile',</v>
+        <v>) ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='User';</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F46" s="10"/>
+      <c r="A46" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="G46" s="15" t="str">
         <f>IF(
     A46="Column",
@@ -3421,10 +3424,26 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `salt` varchar(100)  COMMENT 'salt code ',</v>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:7">
+      <c r="A47" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="7"/>
       <c r="G47" s="15" t="str">
         <f>IF(
     A47="Column",
@@ -3462,10 +3481,22 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   PRIMARY KEY(`id`)</v>
+        <v>CREATE TABLE `dn_user_role` (</v>
       </c>
     </row>
     <row r="48" spans="1:7">
+      <c r="A48" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="10"/>
       <c r="G48" s="15" t="str">
         <f>IF(
     A48="Column",
@@ -3503,10 +3534,22 @@
     ""
     )
 )</f>
-        <v>) ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='User';</v>
+        <v xml:space="preserve">   `id` bigint(19)  NOT NULL  COMMENT 'Pk',</v>
       </c>
     </row>
     <row r="49" spans="1:7">
+      <c r="A49" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F49" s="10"/>
       <c r="G49" s="15" t="str">
         <f>IF(
     A49="Column",
@@ -3544,19 +3587,24 @@
     ""
     )
 )</f>
-        <v/>
+        <v xml:space="preserve">   `user_id` bigint(19)  NOT NULL  COMMENT 'user id',</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="A50" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F50" s="10"/>
       <c r="G50" s="15" t="str">
         <f>IF(
     A50="Column",
@@ -3594,26 +3642,10 @@
     ""
     )
 )</f>
-        <v/>
+        <v xml:space="preserve">   `role_id` bigint(19)  COMMENT 'role id',</v>
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="7"/>
       <c r="G51" s="15" t="str">
         <f>IF(
     A51="Column",
@@ -3651,22 +3683,10 @@
     ""
     )
 )</f>
-        <v>CREATE TABLE `user_role` (</v>
+        <v xml:space="preserve">   PRIMARY KEY(`id`)</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" s="10"/>
       <c r="G52" s="15" t="str">
         <f>IF(
     A52="Column",
@@ -3704,22 +3724,10 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `id` bigint(19)  NOT NULL  COMMENT 'Pk',</v>
+        <v>) ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='User Role';</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F53" s="10"/>
       <c r="G53" s="15" t="str">
         <f>IF(
     A53="Column",
@@ -3757,24 +3765,10 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `user_id` bigint(19)  NOT NULL  COMMENT 'user id',</v>
+        <v/>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="9"/>
-      <c r="E54" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F54" s="10"/>
       <c r="G54" s="15" t="str">
         <f>IF(
     A54="Column",
@@ -3812,7 +3806,7 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   `role_id` bigint(19)  COMMENT 'role id',</v>
+        <v/>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -3853,7 +3847,7 @@
     ""
     )
 )</f>
-        <v xml:space="preserve">   PRIMARY KEY(`id`)</v>
+        <v/>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3894,7 +3888,7 @@
     ""
     )
 )</f>
-        <v>) ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='User Role';</v>
+        <v/>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -6924,170 +6918,6 @@
         AND( A130="", A129&lt;&gt;""),
         "   PRIMARY KEY(`"
             &amp; LOOKUP(1,0/($E$4:E129="Pk"),$A$4:A129)
-                &amp; "`)",
-    ""
-    )
-)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="131" spans="7:7">
-      <c r="G131" s="15" t="str">
-        <f>IF(
-    A131="Column",
-    "CREATE TABLE `"
-        &amp; LOOKUP(1,0/($A$4:A131="Table"),$B$4:B131)
-            &amp; "` (",
-    ""
-)
-&amp;
-IF(
-    AND( A130="", A129&lt;&gt;"", A127&lt;&gt;""),
-    ") ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='"
-        &amp; LOOKUP(1,0/($A$4:A130="Table"),$C$4:C130)
-            &amp; "';",
-    ""
-)
-&amp;
-IF(
-    AND( A131&lt;&gt;"", A131&lt;&gt;"Table", A131&lt;&gt;"Column"),
-    (
-        "   `" &amp; A131
-            &amp;"` " &amp; B131
-            &amp; " " &amp; IF(C131="y",""," NOT NULL ")
-            &amp; IF(D131&lt;&gt;""," DEFAULT " &amp; D131 &amp;"","")
-            &amp;" COMMENT '" &amp; E131 &amp;"',"),
-    ""
-)
-&amp;
-(
-    IF(
-        AND( A131="", A130&lt;&gt;""),
-        "   PRIMARY KEY(`"
-            &amp; LOOKUP(1,0/($E$4:E130="Pk"),$A$4:A130)
-                &amp; "`)",
-    ""
-    )
-)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="132" spans="7:7">
-      <c r="G132" s="15" t="str">
-        <f>IF(
-    A132="Column",
-    "CREATE TABLE `"
-        &amp; LOOKUP(1,0/($A$4:A132="Table"),$B$4:B132)
-            &amp; "` (",
-    ""
-)
-&amp;
-IF(
-    AND( A131="", A130&lt;&gt;"", A128&lt;&gt;""),
-    ") ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='"
-        &amp; LOOKUP(1,0/($A$4:A131="Table"),$C$4:C131)
-            &amp; "';",
-    ""
-)
-&amp;
-IF(
-    AND( A132&lt;&gt;"", A132&lt;&gt;"Table", A132&lt;&gt;"Column"),
-    (
-        "   `" &amp; A132
-            &amp;"` " &amp; B132
-            &amp; " " &amp; IF(C132="y",""," NOT NULL ")
-            &amp; IF(D132&lt;&gt;""," DEFAULT " &amp; D132 &amp;"","")
-            &amp;" COMMENT '" &amp; E132 &amp;"',"),
-    ""
-)
-&amp;
-(
-    IF(
-        AND( A132="", A131&lt;&gt;""),
-        "   PRIMARY KEY(`"
-            &amp; LOOKUP(1,0/($E$4:E131="Pk"),$A$4:A131)
-                &amp; "`)",
-    ""
-    )
-)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="133" spans="7:7">
-      <c r="G133" s="15" t="str">
-        <f>IF(
-    A133="Column",
-    "CREATE TABLE `"
-        &amp; LOOKUP(1,0/($A$4:A133="Table"),$B$4:B133)
-            &amp; "` (",
-    ""
-)
-&amp;
-IF(
-    AND( A132="", A131&lt;&gt;"", A129&lt;&gt;""),
-    ") ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='"
-        &amp; LOOKUP(1,0/($A$4:A132="Table"),$C$4:C132)
-            &amp; "';",
-    ""
-)
-&amp;
-IF(
-    AND( A133&lt;&gt;"", A133&lt;&gt;"Table", A133&lt;&gt;"Column"),
-    (
-        "   `" &amp; A133
-            &amp;"` " &amp; B133
-            &amp; " " &amp; IF(C133="y",""," NOT NULL ")
-            &amp; IF(D133&lt;&gt;""," DEFAULT " &amp; D133 &amp;"","")
-            &amp;" COMMENT '" &amp; E133 &amp;"',"),
-    ""
-)
-&amp;
-(
-    IF(
-        AND( A133="", A132&lt;&gt;""),
-        "   PRIMARY KEY(`"
-            &amp; LOOKUP(1,0/($E$4:E132="Pk"),$A$4:A132)
-                &amp; "`)",
-    ""
-    )
-)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="134" spans="7:7">
-      <c r="G134" s="15" t="str">
-        <f>IF(
-    A134="Column",
-    "CREATE TABLE `"
-        &amp; LOOKUP(1,0/($A$4:A134="Table"),$B$4:B134)
-            &amp; "` (",
-    ""
-)
-&amp;
-IF(
-    AND( A133="", A132&lt;&gt;"", A130&lt;&gt;""),
-    ") ENGINE=InnoDB DEFAULT CHARSET=utf8mb4 COMMENT='"
-        &amp; LOOKUP(1,0/($A$4:A133="Table"),$C$4:C133)
-            &amp; "';",
-    ""
-)
-&amp;
-IF(
-    AND( A134&lt;&gt;"", A134&lt;&gt;"Table", A134&lt;&gt;"Column"),
-    (
-        "   `" &amp; A134
-            &amp;"` " &amp; B134
-            &amp; " " &amp; IF(C134="y",""," NOT NULL ")
-            &amp; IF(D134&lt;&gt;""," DEFAULT " &amp; D134 &amp;"","")
-            &amp;" COMMENT '" &amp; E134 &amp;"',"),
-    ""
-)
-&amp;
-(
-    IF(
-        AND( A134="", A133&lt;&gt;""),
-        "   PRIMARY KEY(`"
-            &amp; LOOKUP(1,0/($E$4:E133="Pk"),$A$4:A133)
                 &amp; "`)",
     ""
     )
@@ -7109,8 +6939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087F83DC-8F46-A246-9277-ED010621A32D}">
   <dimension ref="A1:AC58"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7174,53 +7004,53 @@
     </row>
     <row r="2" spans="1:29" ht="40" customHeight="1">
       <c r="A2" s="20" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="18" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U2" s="22" t="str">
         <f>"'"</f>
@@ -7245,7 +7075,7 @@
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
@@ -7289,15 +7119,15 @@
         <v>null</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q3" s="19" t="str">
         <f>"null"</f>
         <v>null</v>
       </c>
       <c r="S3" s="23" t="str">
-        <f>"insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values("</f>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <f>"insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values("</f>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T3" s="23" t="str">
         <f>I3&amp;$R$1</f>
@@ -7343,12 +7173,12 @@
     <row r="4" spans="1:29">
       <c r="A4" s="19"/>
       <c r="B4" s="21" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19">
@@ -7388,15 +7218,15 @@
         <v>1908032303000000001</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q4" s="19" t="str">
         <f t="shared" ref="Q4:Q58" si="6">"null"</f>
         <v>null</v>
       </c>
       <c r="S4" s="23" t="str">
-        <f t="shared" ref="S4:S58" si="7">"insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values("</f>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <f t="shared" ref="S4:S58" si="7">"insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values("</f>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T4" s="23" t="str">
         <f t="shared" ref="T4:T58" si="8">I4&amp;$R$1</f>
@@ -7443,12 +7273,12 @@
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="21" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G5" s="19">
         <v>2</v>
@@ -7487,7 +7317,7 @@
         <v>1908032303000000002</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q5" s="19" t="str">
         <f t="shared" si="6"/>
@@ -7495,7 +7325,7 @@
       </c>
       <c r="S5" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T5" s="23" t="str">
         <f t="shared" si="8"/>
@@ -7542,12 +7372,12 @@
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="21" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G6" s="19">
         <v>2</v>
@@ -7586,7 +7416,7 @@
         <v>1908032303000000002</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q6" s="19" t="str">
         <f t="shared" si="6"/>
@@ -7594,7 +7424,7 @@
       </c>
       <c r="S6" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T6" s="23" t="str">
         <f t="shared" si="8"/>
@@ -7641,12 +7471,12 @@
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="21" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G7" s="19">
         <v>2</v>
@@ -7685,7 +7515,7 @@
         <v>1908032303000000002</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q7" s="19" t="str">
         <f t="shared" si="6"/>
@@ -7693,7 +7523,7 @@
       </c>
       <c r="S7" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T7" s="23" t="str">
         <f t="shared" si="8"/>
@@ -7739,12 +7569,12 @@
     <row r="8" spans="1:29">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19">
@@ -7784,7 +7614,7 @@
         <v>1908032303000000001</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q8" s="19" t="str">
         <f t="shared" si="6"/>
@@ -7792,7 +7622,7 @@
       </c>
       <c r="S8" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T8" s="23" t="str">
         <f t="shared" si="8"/>
@@ -7839,12 +7669,12 @@
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
       <c r="F9" s="19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G9" s="19">
         <v>2</v>
@@ -7883,7 +7713,7 @@
         <v>1908032303000000006</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q9" s="19" t="str">
         <f t="shared" si="6"/>
@@ -7891,7 +7721,7 @@
       </c>
       <c r="S9" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T9" s="23" t="str">
         <f t="shared" si="8"/>
@@ -7938,12 +7768,12 @@
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G10" s="19">
         <v>2</v>
@@ -7982,7 +7812,7 @@
         <v>1908032303000000006</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q10" s="19" t="str">
         <f t="shared" si="6"/>
@@ -7990,7 +7820,7 @@
       </c>
       <c r="S10" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T10" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8037,12 +7867,12 @@
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
       <c r="F11" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G11" s="19">
         <v>2</v>
@@ -8081,7 +7911,7 @@
         <v>1908032303000000006</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q11" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8089,7 +7919,7 @@
       </c>
       <c r="S11" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T11" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8136,12 +7966,12 @@
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G12" s="19">
         <v>2</v>
@@ -8180,7 +8010,7 @@
         <v>1908032303000000006</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q12" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8188,7 +8018,7 @@
       </c>
       <c r="S12" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T12" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8235,12 +8065,12 @@
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G13" s="19">
         <v>2</v>
@@ -8279,7 +8109,7 @@
         <v>1908032303000000006</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q13" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8287,7 +8117,7 @@
       </c>
       <c r="S13" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T13" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8334,12 +8164,12 @@
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G14" s="19">
         <v>2</v>
@@ -8378,7 +8208,7 @@
         <v>1908032303000000006</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q14" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8386,7 +8216,7 @@
       </c>
       <c r="S14" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T14" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8432,12 +8262,12 @@
     <row r="15" spans="1:29">
       <c r="A15" s="19"/>
       <c r="B15" s="19" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19">
@@ -8477,7 +8307,7 @@
         <v>1908032303000000001</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q15" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8485,7 +8315,7 @@
       </c>
       <c r="S15" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T15" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8532,12 +8362,12 @@
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
       <c r="F16" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G16" s="19">
         <v>2</v>
@@ -8576,7 +8406,7 @@
         <v>1908032303000000013</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q16" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8584,7 +8414,7 @@
       </c>
       <c r="S16" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T16" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8631,12 +8461,12 @@
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G17" s="19">
         <v>2</v>
@@ -8675,7 +8505,7 @@
         <v>1908032303000000013</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q17" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8683,7 +8513,7 @@
       </c>
       <c r="S17" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T17" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8730,12 +8560,12 @@
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G18" s="19">
         <v>2</v>
@@ -8774,7 +8604,7 @@
         <v>1908032303000000013</v>
       </c>
       <c r="P18" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q18" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8782,7 +8612,7 @@
       </c>
       <c r="S18" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T18" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8829,12 +8659,12 @@
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G19" s="19">
         <v>2</v>
@@ -8873,7 +8703,7 @@
         <v>1908032303000000013</v>
       </c>
       <c r="P19" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q19" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8881,7 +8711,7 @@
       </c>
       <c r="S19" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T19" s="23" t="str">
         <f t="shared" si="8"/>
@@ -8928,12 +8758,12 @@
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G20" s="19">
         <v>2</v>
@@ -8972,7 +8802,7 @@
         <v>1908032303000000013</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q20" s="19" t="str">
         <f t="shared" si="6"/>
@@ -8980,7 +8810,7 @@
       </c>
       <c r="S20" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T20" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9027,12 +8857,12 @@
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G21" s="19">
         <v>2</v>
@@ -9071,7 +8901,7 @@
         <v>1908032303000000013</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q21" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9079,7 +8909,7 @@
       </c>
       <c r="S21" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T21" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9126,12 +8956,12 @@
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G22" s="19">
         <v>2</v>
@@ -9170,7 +9000,7 @@
         <v>1908032303000000013</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q22" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9178,7 +9008,7 @@
       </c>
       <c r="S22" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T22" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9225,12 +9055,12 @@
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G23" s="19">
         <v>2</v>
@@ -9269,7 +9099,7 @@
         <v>1908032303000000013</v>
       </c>
       <c r="P23" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q23" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9277,7 +9107,7 @@
       </c>
       <c r="S23" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T23" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9324,12 +9154,12 @@
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
       <c r="F24" s="19" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G24" s="19">
         <v>2</v>
@@ -9368,7 +9198,7 @@
         <v>1908032303000000013</v>
       </c>
       <c r="P24" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q24" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9376,7 +9206,7 @@
       </c>
       <c r="S24" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T24" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9422,12 +9252,12 @@
     <row r="25" spans="1:29">
       <c r="A25" s="19"/>
       <c r="B25" s="19" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19">
@@ -9467,7 +9297,7 @@
         <v>1908032303000000001</v>
       </c>
       <c r="P25" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q25" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9475,7 +9305,7 @@
       </c>
       <c r="S25" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T25" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9522,12 +9352,12 @@
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="19" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G26" s="19">
         <v>2</v>
@@ -9566,7 +9396,7 @@
         <v>1908032303000000023</v>
       </c>
       <c r="P26" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q26" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9574,7 +9404,7 @@
       </c>
       <c r="S26" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T26" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9621,12 +9451,12 @@
       <c r="A27" s="19"/>
       <c r="B27" s="19"/>
       <c r="C27" s="19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G27" s="19">
         <v>2</v>
@@ -9665,7 +9495,7 @@
         <v>1908032303000000023</v>
       </c>
       <c r="P27" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q27" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9673,7 +9503,7 @@
       </c>
       <c r="S27" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T27" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9719,12 +9549,12 @@
     <row r="28" spans="1:29">
       <c r="A28" s="19"/>
       <c r="B28" s="19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="21" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="19">
@@ -9764,7 +9594,7 @@
         <v>1908032303000000001</v>
       </c>
       <c r="P28" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q28" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9772,7 +9602,7 @@
       </c>
       <c r="S28" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T28" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9819,12 +9649,12 @@
       <c r="A29" s="19"/>
       <c r="B29" s="19"/>
       <c r="C29" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G29" s="19">
         <v>2</v>
@@ -9863,7 +9693,7 @@
         <v>1908032303000000026</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q29" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9871,7 +9701,7 @@
       </c>
       <c r="S29" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T29" s="23" t="str">
         <f t="shared" si="8"/>
@@ -9918,12 +9748,12 @@
       <c r="A30" s="19"/>
       <c r="B30" s="19"/>
       <c r="C30" s="19" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G30" s="19">
         <v>2</v>
@@ -9962,7 +9792,7 @@
         <v>1908032303000000026</v>
       </c>
       <c r="P30" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q30" s="19" t="str">
         <f t="shared" si="6"/>
@@ -9970,7 +9800,7 @@
       </c>
       <c r="S30" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T30" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10017,12 +9847,12 @@
       <c r="A31" s="19"/>
       <c r="B31" s="19"/>
       <c r="C31" s="19" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G31" s="19">
         <v>2</v>
@@ -10061,7 +9891,7 @@
         <v>1908032303000000026</v>
       </c>
       <c r="P31" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q31" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10069,7 +9899,7 @@
       </c>
       <c r="S31" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T31" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10116,12 +9946,12 @@
       <c r="A32" s="19"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G32" s="19">
         <v>2</v>
@@ -10160,7 +9990,7 @@
         <v>1908032303000000026</v>
       </c>
       <c r="P32" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q32" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10168,7 +9998,7 @@
       </c>
       <c r="S32" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T32" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10215,12 +10045,12 @@
       <c r="A33" s="19"/>
       <c r="B33" s="19"/>
       <c r="C33" s="19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G33" s="19">
         <v>2</v>
@@ -10259,7 +10089,7 @@
         <v>1908032303000000026</v>
       </c>
       <c r="P33" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q33" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10267,7 +10097,7 @@
       </c>
       <c r="S33" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T33" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10313,12 +10143,12 @@
     <row r="34" spans="1:29">
       <c r="A34" s="19"/>
       <c r="B34" s="19" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F34" s="19"/>
       <c r="G34" s="19">
@@ -10358,7 +10188,7 @@
         <v>1908032303000000001</v>
       </c>
       <c r="P34" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q34" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10366,7 +10196,7 @@
       </c>
       <c r="S34" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T34" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10413,12 +10243,12 @@
       <c r="A35" s="19"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G35" s="19">
         <v>2</v>
@@ -10457,7 +10287,7 @@
         <v>1908032303000000032</v>
       </c>
       <c r="P35" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q35" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10465,7 +10295,7 @@
       </c>
       <c r="S35" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T35" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10512,12 +10342,12 @@
       <c r="A36" s="19"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G36" s="19">
         <v>2</v>
@@ -10556,7 +10386,7 @@
         <v>1908032303000000032</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q36" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10564,7 +10394,7 @@
       </c>
       <c r="S36" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T36" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10609,7 +10439,7 @@
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="19" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -10653,7 +10483,7 @@
         <v>null</v>
       </c>
       <c r="P37" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q37" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10661,7 +10491,7 @@
       </c>
       <c r="S37" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T37" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10707,12 +10537,12 @@
     <row r="38" spans="1:29">
       <c r="A38" s="19"/>
       <c r="B38" s="19" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
       <c r="E38" s="19" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F38" s="19"/>
       <c r="G38" s="19">
@@ -10752,7 +10582,7 @@
         <v>1908032303000000035</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q38" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10760,7 +10590,7 @@
       </c>
       <c r="S38" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T38" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10807,12 +10637,12 @@
       <c r="A39" s="19"/>
       <c r="B39" s="19"/>
       <c r="C39" s="19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
       <c r="F39" s="19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G39" s="19">
         <v>2</v>
@@ -10851,7 +10681,7 @@
         <v>1908032303000000036</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q39" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10859,7 +10689,7 @@
       </c>
       <c r="S39" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T39" s="23" t="str">
         <f t="shared" si="8"/>
@@ -10906,12 +10736,12 @@
       <c r="A40" s="19"/>
       <c r="B40" s="19"/>
       <c r="C40" s="19" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
       <c r="F40" s="19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G40" s="19">
         <v>2</v>
@@ -10950,7 +10780,7 @@
         <v>1908032303000000036</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q40" s="19" t="str">
         <f t="shared" si="6"/>
@@ -10958,7 +10788,7 @@
       </c>
       <c r="S40" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T40" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11005,12 +10835,12 @@
       <c r="A41" s="19"/>
       <c r="B41" s="19"/>
       <c r="C41" s="19" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="19"/>
       <c r="F41" s="19" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G41" s="19">
         <v>2</v>
@@ -11049,7 +10879,7 @@
         <v>1908032303000000036</v>
       </c>
       <c r="P41" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q41" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11057,7 +10887,7 @@
       </c>
       <c r="S41" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T41" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11104,12 +10934,12 @@
       <c r="A42" s="19"/>
       <c r="B42" s="19"/>
       <c r="C42" s="19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
       <c r="F42" s="19" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G42" s="19">
         <v>2</v>
@@ -11148,7 +10978,7 @@
         <v>1908032303000000036</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q42" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11156,7 +10986,7 @@
       </c>
       <c r="S42" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T42" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11203,12 +11033,12 @@
       <c r="A43" s="19"/>
       <c r="B43" s="19"/>
       <c r="C43" s="19" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="19"/>
       <c r="F43" s="19" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G43" s="19">
         <v>2</v>
@@ -11247,7 +11077,7 @@
         <v>1908032303000000036</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q43" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11255,7 +11085,7 @@
       </c>
       <c r="S43" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T43" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11301,12 +11131,12 @@
     <row r="44" spans="1:29">
       <c r="A44" s="19"/>
       <c r="B44" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
       <c r="E44" s="19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F44" s="19"/>
       <c r="G44" s="19">
@@ -11346,7 +11176,7 @@
         <v>1908032303000000035</v>
       </c>
       <c r="P44" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q44" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11354,7 +11184,7 @@
       </c>
       <c r="S44" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T44" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11401,12 +11231,12 @@
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
       <c r="C45" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="19"/>
       <c r="F45" s="19" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G45" s="19">
         <v>2</v>
@@ -11445,7 +11275,7 @@
         <v>1908032303000000042</v>
       </c>
       <c r="P45" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q45" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11453,7 +11283,7 @@
       </c>
       <c r="S45" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T45" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11500,12 +11330,12 @@
       <c r="A46" s="19"/>
       <c r="B46" s="19"/>
       <c r="C46" s="19" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="19"/>
       <c r="F46" s="19" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G46" s="19">
         <v>2</v>
@@ -11544,7 +11374,7 @@
         <v>1908032303000000042</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q46" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11552,7 +11382,7 @@
       </c>
       <c r="S46" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T46" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11599,12 +11429,12 @@
       <c r="A47" s="19"/>
       <c r="B47" s="19"/>
       <c r="C47" s="19" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="19"/>
       <c r="F47" s="19" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G47" s="19">
         <v>2</v>
@@ -11643,7 +11473,7 @@
         <v>1908032303000000042</v>
       </c>
       <c r="P47" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q47" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11651,7 +11481,7 @@
       </c>
       <c r="S47" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T47" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11698,12 +11528,12 @@
       <c r="A48" s="19"/>
       <c r="B48" s="19"/>
       <c r="C48" s="19" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="19"/>
       <c r="F48" s="19" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G48" s="19">
         <v>2</v>
@@ -11742,7 +11572,7 @@
         <v>1908032303000000042</v>
       </c>
       <c r="P48" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q48" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11750,7 +11580,7 @@
       </c>
       <c r="S48" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T48" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11797,12 +11627,12 @@
       <c r="A49" s="19"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
       <c r="F49" s="19" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G49" s="19">
         <v>2</v>
@@ -11841,7 +11671,7 @@
         <v>1908032303000000042</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q49" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11849,7 +11679,7 @@
       </c>
       <c r="S49" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T49" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11896,12 +11726,12 @@
       <c r="A50" s="19"/>
       <c r="B50" s="19"/>
       <c r="C50" s="19" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D50" s="19"/>
       <c r="E50" s="19"/>
       <c r="F50" s="19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G50" s="19">
         <v>2</v>
@@ -11940,7 +11770,7 @@
         <v>1908032303000000042</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q50" s="19" t="str">
         <f t="shared" si="6"/>
@@ -11948,7 +11778,7 @@
       </c>
       <c r="S50" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T50" s="23" t="str">
         <f t="shared" si="8"/>
@@ -11994,12 +11824,12 @@
     <row r="51" spans="1:29">
       <c r="A51" s="19"/>
       <c r="B51" s="19" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
       <c r="E51" s="19" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F51" s="19"/>
       <c r="G51" s="19">
@@ -12039,7 +11869,7 @@
         <v>1908032303000000035</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q51" s="19" t="str">
         <f t="shared" si="6"/>
@@ -12047,7 +11877,7 @@
       </c>
       <c r="S51" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T51" s="23" t="str">
         <f t="shared" si="8"/>
@@ -12094,12 +11924,12 @@
       <c r="A52" s="19"/>
       <c r="B52" s="19"/>
       <c r="C52" s="19" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
       <c r="F52" s="19" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G52" s="19">
         <v>2</v>
@@ -12138,7 +11968,7 @@
         <v>1908032303000000049</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q52" s="19" t="str">
         <f t="shared" si="6"/>
@@ -12146,7 +11976,7 @@
       </c>
       <c r="S52" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T52" s="23" t="str">
         <f t="shared" si="8"/>
@@ -12193,7 +12023,7 @@
       <c r="A53" s="19"/>
       <c r="B53" s="19"/>
       <c r="C53" s="19" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="19"/>
@@ -12235,7 +12065,7 @@
         <v>1908032303000000049</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q53" s="19" t="str">
         <f t="shared" si="6"/>
@@ -12243,7 +12073,7 @@
       </c>
       <c r="S53" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T53" s="23" t="str">
         <f t="shared" si="8"/>
@@ -12291,11 +12121,11 @@
       <c r="B54" s="19"/>
       <c r="C54" s="19"/>
       <c r="D54" s="19" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E54" s="19"/>
       <c r="F54" s="19" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G54" s="19">
         <v>3</v>
@@ -12334,7 +12164,7 @@
         <v>1908032303000000051</v>
       </c>
       <c r="P54" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q54" s="19" t="str">
         <f t="shared" si="6"/>
@@ -12342,7 +12172,7 @@
       </c>
       <c r="S54" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T54" s="23" t="str">
         <f t="shared" si="8"/>
@@ -12390,11 +12220,11 @@
       <c r="B55" s="19"/>
       <c r="C55" s="19"/>
       <c r="D55" s="19" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E55" s="19"/>
       <c r="F55" s="19" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G55" s="19">
         <v>3</v>
@@ -12433,7 +12263,7 @@
         <v>1908032303000000051</v>
       </c>
       <c r="P55" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q55" s="19" t="str">
         <f t="shared" si="6"/>
@@ -12441,7 +12271,7 @@
       </c>
       <c r="S55" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T55" s="23" t="str">
         <f t="shared" si="8"/>
@@ -12489,11 +12319,11 @@
       <c r="B56" s="19"/>
       <c r="C56" s="19"/>
       <c r="D56" s="19" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E56" s="19"/>
       <c r="F56" s="19" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G56" s="19">
         <v>3</v>
@@ -12532,7 +12362,7 @@
         <v>1908032303000000051</v>
       </c>
       <c r="P56" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q56" s="19" t="str">
         <f t="shared" si="6"/>
@@ -12540,7 +12370,7 @@
       </c>
       <c r="S56" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T56" s="23" t="str">
         <f t="shared" si="8"/>
@@ -12587,12 +12417,12 @@
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="19" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="19"/>
       <c r="F57" s="19" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G57" s="19">
         <v>3</v>
@@ -12631,7 +12461,7 @@
         <v>1908032303000000051</v>
       </c>
       <c r="P57" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q57" s="19" t="str">
         <f t="shared" si="6"/>
@@ -12639,7 +12469,7 @@
       </c>
       <c r="S57" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T57" s="23" t="str">
         <f t="shared" si="8"/>
@@ -12684,13 +12514,13 @@
     </row>
     <row r="58" spans="1:29">
       <c r="A58" s="19" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
       <c r="E58" s="19" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F58" s="19"/>
       <c r="G58" s="19">
@@ -12730,7 +12560,7 @@
         <v>1908032303000000035</v>
       </c>
       <c r="P58" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q58" s="19" t="str">
         <f t="shared" si="6"/>
@@ -12738,7 +12568,7 @@
       </c>
       <c r="S58" s="23" t="str">
         <f t="shared" si="7"/>
-        <v>insert into  permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
+        <v>insert into  dn_permission(id,`name`,fa,url,lev,sort,parent_id,site_code,remark) values(</v>
       </c>
       <c r="T58" s="23" t="str">
         <f t="shared" si="8"/>
@@ -12792,7 +12622,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12808,22 +12638,22 @@
   <sheetData>
     <row r="1" spans="1:15" ht="22" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>33</v>
-      </c>
       <c r="F1" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="24"/>
       <c r="H1" t="str">
@@ -12857,25 +12687,25 @@
         <v>1908040851000000001</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D2" t="str">
         <f>"null"</f>
         <v>null</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="E2:F3" si="0">"null"</f>
         <v>null</v>
       </c>
       <c r="H2" s="27" t="str">
-        <f>"insert into role(id,role_name,role_code,parent_id,role_type,remark) values("</f>
-        <v>insert into role(id,role_name,role_code,parent_id,role_type,remark) values(</v>
+        <f>"insert into dn_role(id,role_name,role_code,parent_id,role_type,remark) values("</f>
+        <v>insert into dn_role(id,role_name,role_code,parent_id,role_type,remark) values(</v>
       </c>
       <c r="I2" s="27" t="str">
         <f>A2 &amp; $H$1</f>
@@ -12912,10 +12742,10 @@
         <v>1908040851000000002</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D3" t="str">
         <f>"null"</f>
@@ -12930,8 +12760,8 @@
         <v>null</v>
       </c>
       <c r="H3" s="27" t="str">
-        <f>"insert into role(id,role_name,role_code,parent_id,role_type,remark) values("</f>
-        <v>insert into role(id,role_name,role_code,parent_id,role_type,remark) values(</v>
+        <f>"insert into dn_role(id,role_name,role_code,parent_id,role_type,remark) values("</f>
+        <v>insert into dn_role(id,role_name,role_code,parent_id,role_type,remark) values(</v>
       </c>
       <c r="I3" s="27" t="str">
         <f>A3 &amp; $H$1</f>
@@ -12972,8 +12802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75A2BD4-C344-954B-B045-8E7E3DA3EDC1}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:L114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12999,31 +12829,31 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -13048,8 +12878,8 @@
         <v>dubbo-nacos-consumer</v>
       </c>
       <c r="G3" s="27" t="str">
-        <f>"insert into role_permission(id,role_id,permission_id,site_code) values("</f>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <f>"insert into dn_role_permission(id,role_id,permission_id,site_code) values("</f>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H3" s="27" t="str">
         <f>CONCATENATE("1908040853",TEXT(ROW()-2,"000000000")) &amp; $F$1</f>
@@ -13094,8 +12924,8 @@
         <v>dubbo-nacos-consumer</v>
       </c>
       <c r="G4" s="27" t="str">
-        <f t="shared" ref="G4:G66" si="0">"insert into role_permission(id,role_id,permission_id,site_code) values("</f>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <f t="shared" ref="G4:G67" si="0">"insert into dn_role_permission(id,role_id,permission_id,site_code) values("</f>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H4" s="27" t="str">
         <f t="shared" ref="H4:H67" si="1">CONCATENATE("1908040853",TEXT(ROW()-2,"000000000")) &amp; $F$1</f>
@@ -13141,7 +12971,7 @@
       </c>
       <c r="G5" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H5" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13187,7 +13017,7 @@
       </c>
       <c r="G6" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H6" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13233,7 +13063,7 @@
       </c>
       <c r="G7" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H7" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13279,7 +13109,7 @@
       </c>
       <c r="G8" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H8" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13325,7 +13155,7 @@
       </c>
       <c r="G9" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H9" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13371,7 +13201,7 @@
       </c>
       <c r="G10" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H10" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13417,7 +13247,7 @@
       </c>
       <c r="G11" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H11" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13463,7 +13293,7 @@
       </c>
       <c r="G12" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H12" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13509,7 +13339,7 @@
       </c>
       <c r="G13" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H13" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13555,7 +13385,7 @@
       </c>
       <c r="G14" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H14" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13601,7 +13431,7 @@
       </c>
       <c r="G15" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H15" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13647,7 +13477,7 @@
       </c>
       <c r="G16" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H16" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13693,7 +13523,7 @@
       </c>
       <c r="G17" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H17" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13739,7 +13569,7 @@
       </c>
       <c r="G18" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H18" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13785,7 +13615,7 @@
       </c>
       <c r="G19" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H19" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13831,7 +13661,7 @@
       </c>
       <c r="G20" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H20" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13877,7 +13707,7 @@
       </c>
       <c r="G21" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H21" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13923,7 +13753,7 @@
       </c>
       <c r="G22" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H22" s="27" t="str">
         <f t="shared" si="1"/>
@@ -13969,7 +13799,7 @@
       </c>
       <c r="G23" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H23" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14015,7 +13845,7 @@
       </c>
       <c r="G24" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H24" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14061,7 +13891,7 @@
       </c>
       <c r="G25" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H25" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14107,7 +13937,7 @@
       </c>
       <c r="G26" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H26" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14153,7 +13983,7 @@
       </c>
       <c r="G27" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H27" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14199,7 +14029,7 @@
       </c>
       <c r="G28" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H28" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14245,7 +14075,7 @@
       </c>
       <c r="G29" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H29" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14291,7 +14121,7 @@
       </c>
       <c r="G30" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H30" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14337,7 +14167,7 @@
       </c>
       <c r="G31" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H31" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14383,7 +14213,7 @@
       </c>
       <c r="G32" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H32" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14429,7 +14259,7 @@
       </c>
       <c r="G33" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H33" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14475,7 +14305,7 @@
       </c>
       <c r="G34" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H34" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14521,7 +14351,7 @@
       </c>
       <c r="G35" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H35" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14567,7 +14397,7 @@
       </c>
       <c r="G36" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H36" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14613,7 +14443,7 @@
       </c>
       <c r="G37" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H37" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14659,7 +14489,7 @@
       </c>
       <c r="G38" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H38" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14705,7 +14535,7 @@
       </c>
       <c r="G39" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H39" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14751,7 +14581,7 @@
       </c>
       <c r="G40" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H40" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14797,7 +14627,7 @@
       </c>
       <c r="G41" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H41" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14843,7 +14673,7 @@
       </c>
       <c r="G42" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H42" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14889,7 +14719,7 @@
       </c>
       <c r="G43" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H43" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14935,7 +14765,7 @@
       </c>
       <c r="G44" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H44" s="27" t="str">
         <f t="shared" si="1"/>
@@ -14981,7 +14811,7 @@
       </c>
       <c r="G45" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H45" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15027,7 +14857,7 @@
       </c>
       <c r="G46" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H46" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15073,7 +14903,7 @@
       </c>
       <c r="G47" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H47" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15119,7 +14949,7 @@
       </c>
       <c r="G48" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H48" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15165,7 +14995,7 @@
       </c>
       <c r="G49" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H49" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15211,7 +15041,7 @@
       </c>
       <c r="G50" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H50" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15257,7 +15087,7 @@
       </c>
       <c r="G51" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H51" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15303,7 +15133,7 @@
       </c>
       <c r="G52" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H52" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15349,7 +15179,7 @@
       </c>
       <c r="G53" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H53" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15395,7 +15225,7 @@
       </c>
       <c r="G54" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H54" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15441,7 +15271,7 @@
       </c>
       <c r="G55" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H55" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15487,7 +15317,7 @@
       </c>
       <c r="G56" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H56" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15533,7 +15363,7 @@
       </c>
       <c r="G57" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H57" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15579,7 +15409,7 @@
       </c>
       <c r="G58" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H58" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15625,7 +15455,7 @@
       </c>
       <c r="G59" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H59" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15671,7 +15501,7 @@
       </c>
       <c r="G60" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H60" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15717,7 +15547,7 @@
       </c>
       <c r="G61" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H61" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15763,7 +15593,7 @@
       </c>
       <c r="G62" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H62" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15809,7 +15639,7 @@
       </c>
       <c r="G63" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H63" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15855,7 +15685,7 @@
       </c>
       <c r="G64" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H64" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15901,7 +15731,7 @@
       </c>
       <c r="G65" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H65" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15947,7 +15777,7 @@
       </c>
       <c r="G66" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H66" s="27" t="str">
         <f t="shared" si="1"/>
@@ -15992,8 +15822,8 @@
         <v>dubbo-nacos-consumer</v>
       </c>
       <c r="G67" s="27" t="str">
-        <f t="shared" ref="G67:G114" si="6">"insert into role_permission(id,role_id,permission_id,site_code) values("</f>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <f t="shared" si="0"/>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H67" s="27" t="str">
         <f t="shared" si="1"/>
@@ -16038,8 +15868,8 @@
         <v>dubbo-nacos-consumer</v>
       </c>
       <c r="G68" s="27" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <f t="shared" ref="G68:G114" si="6">"insert into dn_role_permission(id,role_id,permission_id,site_code) values("</f>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H68" s="27" t="str">
         <f t="shared" ref="H68:H114" si="7">CONCATENATE("1908040853",TEXT(ROW()-2,"000000000")) &amp; $F$1</f>
@@ -16085,7 +15915,7 @@
       </c>
       <c r="G69" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H69" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16131,7 +15961,7 @@
       </c>
       <c r="G70" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H70" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16177,7 +16007,7 @@
       </c>
       <c r="G71" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H71" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16223,7 +16053,7 @@
       </c>
       <c r="G72" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H72" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16269,7 +16099,7 @@
       </c>
       <c r="G73" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H73" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16315,7 +16145,7 @@
       </c>
       <c r="G74" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H74" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16361,7 +16191,7 @@
       </c>
       <c r="G75" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H75" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16407,7 +16237,7 @@
       </c>
       <c r="G76" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H76" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16453,7 +16283,7 @@
       </c>
       <c r="G77" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H77" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16499,7 +16329,7 @@
       </c>
       <c r="G78" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H78" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16545,7 +16375,7 @@
       </c>
       <c r="G79" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H79" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16591,7 +16421,7 @@
       </c>
       <c r="G80" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H80" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16637,7 +16467,7 @@
       </c>
       <c r="G81" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H81" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16683,7 +16513,7 @@
       </c>
       <c r="G82" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H82" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16729,7 +16559,7 @@
       </c>
       <c r="G83" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H83" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16775,7 +16605,7 @@
       </c>
       <c r="G84" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H84" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16821,7 +16651,7 @@
       </c>
       <c r="G85" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H85" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16867,7 +16697,7 @@
       </c>
       <c r="G86" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H86" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16913,7 +16743,7 @@
       </c>
       <c r="G87" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H87" s="27" t="str">
         <f t="shared" si="7"/>
@@ -16959,7 +16789,7 @@
       </c>
       <c r="G88" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H88" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17005,7 +16835,7 @@
       </c>
       <c r="G89" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H89" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17051,7 +16881,7 @@
       </c>
       <c r="G90" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H90" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17097,7 +16927,7 @@
       </c>
       <c r="G91" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H91" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17143,7 +16973,7 @@
       </c>
       <c r="G92" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H92" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17189,7 +17019,7 @@
       </c>
       <c r="G93" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H93" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17235,7 +17065,7 @@
       </c>
       <c r="G94" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H94" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17281,7 +17111,7 @@
       </c>
       <c r="G95" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H95" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17327,7 +17157,7 @@
       </c>
       <c r="G96" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H96" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17373,7 +17203,7 @@
       </c>
       <c r="G97" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H97" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17419,7 +17249,7 @@
       </c>
       <c r="G98" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H98" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17465,7 +17295,7 @@
       </c>
       <c r="G99" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H99" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17511,7 +17341,7 @@
       </c>
       <c r="G100" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H100" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17557,7 +17387,7 @@
       </c>
       <c r="G101" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H101" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17603,7 +17433,7 @@
       </c>
       <c r="G102" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H102" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17649,7 +17479,7 @@
       </c>
       <c r="G103" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H103" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17695,7 +17525,7 @@
       </c>
       <c r="G104" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H104" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17741,7 +17571,7 @@
       </c>
       <c r="G105" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H105" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17787,7 +17617,7 @@
       </c>
       <c r="G106" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H106" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17833,7 +17663,7 @@
       </c>
       <c r="G107" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H107" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17879,7 +17709,7 @@
       </c>
       <c r="G108" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H108" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17925,7 +17755,7 @@
       </c>
       <c r="G109" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H109" s="27" t="str">
         <f t="shared" si="7"/>
@@ -17971,7 +17801,7 @@
       </c>
       <c r="G110" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H110" s="27" t="str">
         <f t="shared" si="7"/>
@@ -18017,7 +17847,7 @@
       </c>
       <c r="G111" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H111" s="27" t="str">
         <f t="shared" si="7"/>
@@ -18063,7 +17893,7 @@
       </c>
       <c r="G112" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H112" s="27" t="str">
         <f t="shared" si="7"/>
@@ -18109,7 +17939,7 @@
       </c>
       <c r="G113" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H113" s="27" t="str">
         <f t="shared" si="7"/>
@@ -18155,7 +17985,7 @@
       </c>
       <c r="G114" s="27" t="str">
         <f t="shared" si="6"/>
-        <v>insert into role_permission(id,role_id,permission_id,site_code) values(</v>
+        <v>insert into dn_role_permission(id,role_id,permission_id,site_code) values(</v>
       </c>
       <c r="H114" s="27" t="str">
         <f t="shared" si="7"/>

</xml_diff>